<commit_message>
Finish unification of the various different parser types.
Tests run again!
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -66,10 +66,10 @@
     <t xml:space="preserve">English strict</t>
   </si>
   <si>
-    <t xml:space="preserve">Spanish2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portuguese2</t>
+    <t xml:space="preserve">Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portuguese</t>
   </si>
   <si>
     <t xml:space="preserve">French</t>
@@ -237,6 +237,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -475,10 +476,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -516,7 +517,6 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">

</xml_diff>

<commit_message>
Make progress on format guesser
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -424,7 +424,7 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF8D1D75"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -471,15 +471,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF8D1D75"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>

<commit_message>
added (test comments) to cells
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -114,12 +114,6 @@
     <t>un, une</t>
   </si>
   <si>
-    <t>/etakɾã/ [e.ta.'kɾã] (uno; solo){4}; /etakrã/</t>
-  </si>
-  <si>
-    <t>&lt;peteĩ&gt;(uno){Guasch1962:670}</t>
-  </si>
-  <si>
     <t>[petẽˈʔĩ]</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t xml:space="preserve">/gwɨɾa pɨʧã/ [gwɨ.'ɾa pɨ.'ʧa~testvariant] (cuatro){4} </t>
+  </si>
+  <si>
+    <t>/etakɾã/ [e.ta.'kɾã] (uno; solo) (test comment) (test comment 2){4}; /etakrã/</t>
+  </si>
+  <si>
+    <t>&lt;peteĩ&gt;(uno){Guasch1962:670} (Test comment 3)</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -771,20 +771,20 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -800,35 +800,35 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="I5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -841,36 +841,36 @@
     </row>
     <row r="7" spans="1:10" ht="14">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -883,43 +883,43 @@
     </row>
     <row r="9" spans="1:10" ht="14">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -927,27 +927,27 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added (NCP: test procedural comment)
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -114,9 +114,6 @@
     <t>un, une</t>
   </si>
   <si>
-    <t>[petẽˈʔĩ]</t>
-  </si>
-  <si>
     <t>one@</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>&lt;peteĩ&gt;(uno){Guasch1962:670} (Test comment 3)</t>
+  </si>
+  <si>
+    <t>[petẽˈʔĩ] (NPC: Test procedural comment)</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -771,20 +771,20 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -800,35 +800,35 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -841,36 +841,36 @@
     </row>
     <row r="7" spans="1:10" ht="14">
       <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -883,43 +883,43 @@
     </row>
     <row r="9" spans="1:10" ht="14">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -927,27 +927,27 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some nasty special cases for debugging
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -216,13 +216,13 @@
     <t xml:space="preserve">/gwɨɾa pɨʧã/ [gwɨ.'ɾa pɨ.'ʧa~testvariant] (cuatro){4} </t>
   </si>
   <si>
-    <t>/etakɾã/ [e.ta.'kɾã] (uno; solo) (test comment) (test comment 2){4}; /etakrã/</t>
-  </si>
-  <si>
     <t>&lt;peteĩ&gt;(uno){Guasch1962:670} (Test comment 3)</t>
   </si>
   <si>
     <t>[petẽˈʔĩ] (NPC: Test procedural comment)</t>
+  </si>
+  <si>
+    <t>/etakɾã/ [e.ta.'kɾã] ~[test_variant with various comments] (uno; solo) (test comment) (test comment 2){4}; /etakrã/</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -771,14 +771,14 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14">

</xml_diff>

<commit_message>
added some test comments for debugging
</commit_message>
<xml_diff>
--- a/test/data/excel/small.xlsx
+++ b/test/data/excel/small.xlsx
@@ -129,12 +129,6 @@
     <t>deux</t>
   </si>
   <si>
-    <t>&lt;mokõi&gt;(dos){Guasch1962:616}</t>
-  </si>
-  <si>
-    <t>[mõˈkõj̃]</t>
-  </si>
-  <si>
     <t>two@</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t>/etakɾã/ [e.ta.'kɾã] ~[test_variant with various comments] (uno; solo) (test comment) (test comment 2){4}; /etakrã/</t>
+  </si>
+  <si>
+    <t>&lt;mokõi&gt;(dos){Guasch1962:616} (PCP: Test procedural comment lands in variants)</t>
+  </si>
+  <si>
+    <t>[mõˈkõj̃] (PCP: Procedural comment before real comment) (dos)</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -771,14 +771,14 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14">
@@ -813,22 +813,22 @@
         <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -841,36 +841,36 @@
     </row>
     <row r="7" spans="1:10" ht="14">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -883,43 +883,43 @@
     </row>
     <row r="9" spans="1:10" ht="14">
       <c r="A9" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -927,27 +927,27 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>